<commit_message>
test: compliance service integration test
</commit_message>
<xml_diff>
--- a/bc_obps/reporting/tests/service/test_compliance_service/compliance_class_manual_calcs.xlsx
+++ b/bc_obps/reporting/tests/service/test_compliance_service/compliance_class_manual_calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbastian/projects/cas-registration/bc_obps/reporting/tests/service/test_compliance_service/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA856FD-B2E9-C242-95BF-2CC8308609E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BD2286-D439-2946-A251-8CBA4CCB8BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2280" windowWidth="27680" windowHeight="16160" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="39">
   <si>
     <t>Product 1</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>Emission 6</t>
+  </si>
+  <si>
+    <t>GSC / funny category 13</t>
   </si>
 </sst>
 </file>
@@ -164,12 +170,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -184,8 +196,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1413,7 +1426,7 @@
   <dimension ref="A2:H32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J34" sqref="A1:J34"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1752,7 +1765,7 @@
   <dimension ref="A2:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1762,7 +1775,7 @@
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
@@ -1851,6 +1864,15 @@
       <c r="E7">
         <v>0</v>
       </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7">
+        <v>55.55</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
@@ -1865,8 +1887,8 @@
       <c r="D9">
         <v>75000.008799999996</v>
       </c>
-      <c r="E9">
-        <v>0</v>
+      <c r="E9" s="1">
+        <v>2200</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
@@ -1882,8 +1904,8 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10">
-        <v>2200</v>
+      <c r="E10" s="1">
+        <v>55.55</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -2010,11 +2032,11 @@
         <v>75000.008799999996</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>2255.5500000000002</v>
       </c>
       <c r="G27">
         <f>SUM(B27:E27)</f>
-        <v>123001.0577</v>
+        <v>125256.60770000001</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
@@ -2034,11 +2056,11 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>2200</v>
+        <v>55.55</v>
       </c>
       <c r="G28">
         <f t="shared" ref="G28:G32" si="1">SUM(B28:E28)</f>
-        <v>5200.05</v>
+        <v>3055.6000000000004</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
test: adding test case for the excel sheet 6
</commit_message>
<xml_diff>
--- a/bc_obps/reporting/tests/service/test_compliance_service/compliance_class_manual_calcs.xlsx
+++ b/bc_obps/reporting/tests/service/test_compliance_service/compliance_class_manual_calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbastian/projects/cas-registration/bc_obps/reporting/tests/service/test_compliance_service/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319EABA6-A281-7C42-A234-EB6364E55B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD90B857-94BB-C44C-9953-0E43D119D1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33400" yWindow="-28200" windowWidth="51200" windowHeight="26880" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17800" yWindow="-21000" windowWidth="38400" windowHeight="21000" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2208,8 +2208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49CB32B2-CA50-9F42-9C95-A048CB850237}">
   <dimension ref="A2:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2337,10 +2337,10 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="C11">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="D11">
         <v>200</v>
@@ -2426,6 +2426,9 @@
       <c r="C24">
         <v>0.6</v>
       </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
@@ -2439,6 +2442,9 @@
         <f>C24*G4</f>
         <v>6000.03</v>
       </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
@@ -2452,6 +2458,9 @@
         <f>C7-C25</f>
         <v>14000.970800000003</v>
       </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
@@ -2549,20 +2558,20 @@
         <v>26</v>
       </c>
       <c r="B32">
-        <f>SUM((B14*B11)*(B16-((1-(B7/B30))*B17*(B18-2024))))</f>
-        <v>20.88000051999818</v>
+        <f>SUM((B14*B11)*(B16-((1-(B26/B30))*B17*(B18-2024))))</f>
+        <v>2072.0000279999022</v>
       </c>
       <c r="C32">
-        <f>SUM((C14*C11)*(C16-((1-(C7/C30))*C17*(C18-2024))))</f>
-        <v>34.493544919437014</v>
+        <f>SUM((C14*C11)*(C16-((1-(C26/C30))*C17*(C18-2024))))</f>
+        <v>3435.0227898572252</v>
       </c>
       <c r="D32">
-        <f>SUM((D14*D11)*(D16-((1-(D7/D30))*D17*(D18-2024))))</f>
+        <f>SUM((D14*D11)*(D16-((1-(D26/D30))*D17*(D18-2024))))</f>
         <v>136.96</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>192.3335454394352</v>
+        <v>5643.982817857127</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
@@ -2571,11 +2580,11 @@
       </c>
       <c r="B33">
         <f>SUM(B30 - B32)</f>
-        <v>7979.147999480002</v>
+        <v>5928.0279720000981</v>
       </c>
       <c r="C33">
         <f>SUM(C30 - C32)</f>
-        <v>15966.477255080566</v>
+        <v>12565.948010142778</v>
       </c>
       <c r="D33">
         <f>SUM(D30 - D32)</f>
@@ -2583,7 +2592,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>29808.665354560566</v>
+        <v>24357.016082142873</v>
       </c>
       <c r="H33" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
chore: fix naics tightening rate
</commit_message>
<xml_diff>
--- a/bc_obps/reporting/tests/service/test_compliance_service/compliance_class_manual_calcs.xlsx
+++ b/bc_obps/reporting/tests/service/test_compliance_service/compliance_class_manual_calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbastian/projects/cas-registration/bc_obps/reporting/tests/service/test_compliance_service/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD90B857-94BB-C44C-9953-0E43D119D1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1302EBBD-825F-F449-90FE-5017A90933A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17800" yWindow="-21000" windowWidth="38400" windowHeight="21000" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="54">
   <si>
     <t>Product 1</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>&lt;= Total Reporting + compliance emissions computed (should be equal to total emissions reported)</t>
+  </si>
+  <si>
+    <t>Allocated total</t>
   </si>
 </sst>
 </file>
@@ -2209,7 +2212,7 @@
   <dimension ref="A2:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2306,16 +2309,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="B9">
-        <v>12000.048000000001</v>
+        <v>12100.048000000001</v>
       </c>
       <c r="C9">
-        <v>22001.000800000002</v>
+        <v>22101.000800000002</v>
       </c>
       <c r="D9">
-        <v>6000.0001000000002</v>
+        <v>6300.0001000000002</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
@@ -2340,7 +2343,7 @@
         <v>10000</v>
       </c>
       <c r="C11">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="D11">
         <v>200</v>
@@ -2468,19 +2471,19 @@
       </c>
       <c r="B28">
         <f>B9</f>
-        <v>12000.048000000001</v>
+        <v>12100.048000000001</v>
       </c>
       <c r="C28">
         <f>C9</f>
-        <v>22001.000800000002</v>
+        <v>22101.000800000002</v>
       </c>
       <c r="D28">
         <f>D9</f>
-        <v>6000.0001000000002</v>
+        <v>6300.0001000000002</v>
       </c>
       <c r="F28">
         <f t="shared" ref="F28:F33" si="0">SUM(B28:D28)</f>
-        <v>40001.048900000002</v>
+        <v>40501.048900000002</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
@@ -2509,15 +2512,15 @@
         <v>24</v>
       </c>
       <c r="B30">
-        <f>B28-B25</f>
+        <f>B28-B29</f>
         <v>8000.0280000000002</v>
       </c>
       <c r="C30">
-        <f>C28-C25</f>
+        <f>C28-C29</f>
         <v>16000.970800000003</v>
       </c>
       <c r="D30">
-        <f>D28</f>
+        <f>D28-D29</f>
         <v>6000.0001000000002</v>
       </c>
       <c r="F30">
@@ -2563,7 +2566,7 @@
       </c>
       <c r="C32">
         <f>SUM((C14*C11)*(C16-((1-(C26/C30))*C17*(C18-2024))))</f>
-        <v>3435.0227898572252</v>
+        <v>5152.5341847858381</v>
       </c>
       <c r="D32">
         <f>SUM((D14*D11)*(D16-((1-(D26/D30))*D17*(D18-2024))))</f>
@@ -2571,7 +2574,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>5643.982817857127</v>
+        <v>7361.4942127857403</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
@@ -2584,7 +2587,7 @@
       </c>
       <c r="C33">
         <f>SUM(C30 - C32)</f>
-        <v>12565.948010142778</v>
+        <v>10848.436615214165</v>
       </c>
       <c r="D33">
         <f>SUM(D30 - D32)</f>
@@ -2592,7 +2595,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>24357.016082142873</v>
+        <v>22639.504687214263</v>
       </c>
       <c r="H33" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
test: updated compliance tests sheet
</commit_message>
<xml_diff>
--- a/bc_obps/reporting/tests/service/test_compliance_service/compliance_class_manual_calcs.xlsx
+++ b/bc_obps/reporting/tests/service/test_compliance_service/compliance_class_manual_calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbastian/projects/cas-registration/bc_obps/reporting/tests/service/test_compliance_service/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1302EBBD-825F-F449-90FE-5017A90933A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD006F0-B3C0-AA41-9245-EBAC06DD8EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17800" yWindow="-21000" windowWidth="38400" windowHeight="21000" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2211,8 +2211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49CB32B2-CA50-9F42-9C95-A048CB850237}">
   <dimension ref="A2:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2368,7 +2368,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>0.32</v>
+        <v>0.31769999999999998</v>
       </c>
       <c r="C14">
         <v>0.38219999999999998</v>
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B32">
         <f>SUM((B14*B11)*(B16-((1-(B26/B30))*B17*(B18-2024))))</f>
-        <v>2072.0000279999022</v>
+        <v>2057.1075277986529</v>
       </c>
       <c r="C32">
         <f>SUM((C14*C11)*(C16-((1-(C26/C30))*C17*(C18-2024))))</f>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>7361.4942127857403</v>
+        <v>7346.601712584491</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
@@ -2583,7 +2583,7 @@
       </c>
       <c r="B33">
         <f>SUM(B30 - B32)</f>
-        <v>5928.0279720000981</v>
+        <v>5942.9204722013474</v>
       </c>
       <c r="C33">
         <f>SUM(C30 - C32)</f>
@@ -2595,7 +2595,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>22639.504687214263</v>
+        <v>22654.39718741551</v>
       </c>
       <c r="H33" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
chore: updating test for pnp
</commit_message>
<xml_diff>
--- a/bc_obps/reporting/tests/service/test_compliance_service/compliance_class_manual_calcs.xlsx
+++ b/bc_obps/reporting/tests/service/test_compliance_service/compliance_class_manual_calcs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbastian/projects/cas-registration/bc_obps/reporting/tests/service/test_compliance_service/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD006F0-B3C0-AA41-9245-EBAC06DD8EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BBCB3E-238F-9E46-8CCB-B0F09F73AD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17800" yWindow="-21000" windowWidth="38400" windowHeight="21000" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="52">
   <si>
     <t>Product 1</t>
   </si>
@@ -188,21 +188,9 @@
     <t>Total Emission</t>
   </si>
   <si>
-    <t>question whether we include the subtracted overlap in the reporting only</t>
-  </si>
-  <si>
-    <t>biogenic industrial emissions (overlap)</t>
-  </si>
-  <si>
     <t>non-biogenic industrial process</t>
   </si>
   <si>
-    <t>Cam Webster</t>
-  </si>
-  <si>
-    <t>is our contact now for p&amp;p</t>
-  </si>
-  <si>
     <t>Allocated non-industrial reporting only</t>
   </si>
   <si>
@@ -210,6 +198,12 @@
   </si>
   <si>
     <t>Allocated total</t>
+  </si>
+  <si>
+    <t>(chemicals: pure hydrogen peroxide)</t>
+  </si>
+  <si>
+    <t>biogenic industrial emissions (overlap with woody biomass)</t>
   </si>
 </sst>
 </file>
@@ -2209,10 +2203,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49CB32B2-CA50-9F42-9C95-A048CB850237}">
-  <dimension ref="A2:I35"/>
+  <dimension ref="A2:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2249,6 +2243,9 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
       <c r="F3" t="s">
         <v>6</v>
       </c>
@@ -2309,7 +2306,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>12100.048000000001</v>
@@ -2323,7 +2320,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B10">
         <v>100</v>
@@ -2435,7 +2432,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B25">
         <f>G4*B24</f>
@@ -2451,7 +2448,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B26">
         <f>B7-B25</f>
@@ -2532,7 +2529,7 @@
         <v>40501.048900000002</v>
       </c>
       <c r="H30" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
@@ -2577,7 +2574,7 @@
         <v>7346.601712584491</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -2596,17 +2593,6 @@
       <c r="F33">
         <f t="shared" si="0"/>
         <v>22654.39718741551</v>
-      </c>
-      <c r="H33" t="s">
-        <v>49</v>
-      </c>
-      <c r="I33" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B35" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>